<commit_message>
First time use regex, It works better
</commit_message>
<xml_diff>
--- a/parseCOA4Bugget/all.xlsx
+++ b/parseCOA4Bugget/all.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="9495" windowHeight="5160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="12240" windowHeight="8790"/>
   </bookViews>
   <sheets>
     <sheet sheetId="2" name="ALL" state="visible" r:id="rId4"/>
@@ -2139,10 +2139,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="FFFFFF"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="000000"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2400,7 +2400,7 @@
   <dimension ref="A1:H162"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" zoomScale="75" zoomScaleNormal="100">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="9" customHeight="1"/>

</xml_diff>

<commit_message>
Successfully parse and get the transaction data from bank transaction list
</commit_message>
<xml_diff>
--- a/parseCOA4Bugget/all.xlsx
+++ b/parseCOA4Bugget/all.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="12240" windowHeight="8790"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="9495" windowHeight="5160"/>
   </bookViews>
   <sheets>
     <sheet sheetId="2" name="ALL" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'ALL'!$A1:$H162</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'ALL'!$A1:$H167</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="494">
   <si>
     <t>EVA FLIGHT TRAINING ACADEMY</t>
   </si>
@@ -25,7 +25,7 @@
     <t>Non-Routine Report Form</t>
   </si>
   <si>
-    <t>Budget Code: B01</t>
+    <t>Budget Code: B11</t>
   </si>
   <si>
     <t xml:space="preserve">Station: FTA* </t>
@@ -58,7 +58,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Jan.2020~Sep.2020 Actual + Oct.2020~Dec.2020B92</t>
+    <t>Jan.2020~Sep.2020 Actual + Oct.2020~Dec.2020B01</t>
   </si>
   <si>
     <t>Jan.2021~Dec.2021</t>
@@ -457,6 +457,15 @@
     <t>PILOTS EXPENSE-PILOT SIGNING CONTRACT BONUS</t>
   </si>
   <si>
+    <t>5501DF</t>
+  </si>
+  <si>
+    <t>QQ01</t>
+  </si>
+  <si>
+    <t>PILOT TRAVELING EXP.-TRANSPORTATION FEE FOR BUSINESS</t>
+  </si>
+  <si>
     <t>5501EA</t>
   </si>
   <si>
@@ -961,6 +970,15 @@
     <t>TRAVELING EXPENSES-PER DIEM</t>
   </si>
   <si>
+    <t>6204D*</t>
+  </si>
+  <si>
+    <t>TG01</t>
+  </si>
+  <si>
+    <t>TRAVELING EXPENSES-MISCELLANEOUS</t>
+  </si>
+  <si>
     <t>6204F*</t>
   </si>
   <si>
@@ -1024,6 +1042,15 @@
     <t>POSTAGE EXPENSES-LEASED CIRCUIT EXPENSE</t>
   </si>
   <si>
+    <t>6207C*</t>
+  </si>
+  <si>
+    <t>UA01</t>
+  </si>
+  <si>
+    <t>REPAIR &amp; MAINTENANCE-GROUND TRANSPORTATION EQUIPMENT</t>
+  </si>
+  <si>
     <t>6207D*</t>
   </si>
   <si>
@@ -1042,6 +1069,15 @@
     <t>REPAIR &amp; MAINTENANCE-OTHER EQUIPMENT</t>
   </si>
   <si>
+    <t>6209A*</t>
+  </si>
+  <si>
+    <t>UG01</t>
+  </si>
+  <si>
+    <t>UTILITIES EXPENSES-WATER</t>
+  </si>
+  <si>
     <t>6209B*</t>
   </si>
   <si>
@@ -1184,6 +1220,15 @@
   </si>
   <si>
     <t>EMPLOYEE WELFARE-TRANSFER PAYING</t>
+  </si>
+  <si>
+    <t>6219E*</t>
+  </si>
+  <si>
+    <t>VQ05</t>
+  </si>
+  <si>
+    <t>EMPLOYEE WELFARE-MEDICAL EXPENSE</t>
   </si>
   <si>
     <t>6219H*</t>
@@ -2139,50 +2184,50 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFFFF"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -2215,9 +2260,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -2256,162 +2301,186 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H162"/>
+  <dimension ref="A1:H167"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" zoomScale="75" zoomScaleNormal="100">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="9" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="16.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="97.42578125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="16.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="33.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="97.375" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2625,14 +2694,14 @@
         <v>31</v>
       </c>
       <c r="D12" s="29">
-        <v>108710.71</v>
+        <v>5241180.35287</v>
       </c>
       <c r="E12" s="30">
         <v>0</v>
       </c>
       <c r="F12" s="31">
         <f t="shared" si="0"/>
-        <v>-108710.71</v>
+        <v>-5241180.35287</v>
       </c>
       <c r="G12" s="32" t="str">
         <f t="shared" si="1"/>
@@ -2651,14 +2720,14 @@
         <v>34</v>
       </c>
       <c r="D13" s="29">
-        <v>2132747.01</v>
+        <v>3314258.01</v>
       </c>
       <c r="E13" s="30">
         <v>0</v>
       </c>
       <c r="F13" s="31">
         <f t="shared" si="0"/>
-        <v>-2132747.01</v>
+        <v>-3314258.01</v>
       </c>
       <c r="G13" s="32" t="str">
         <f t="shared" si="1"/>
@@ -2677,14 +2746,14 @@
         <v>37</v>
       </c>
       <c r="D14" s="29">
-        <v>57229.94</v>
+        <v>75229.94</v>
       </c>
       <c r="E14" s="30">
         <v>0</v>
       </c>
       <c r="F14" s="31">
         <f t="shared" si="0"/>
-        <v>-57229.94</v>
+        <v>-75229.94</v>
       </c>
       <c r="G14" s="32" t="str">
         <f t="shared" si="1"/>
@@ -2781,14 +2850,14 @@
         <v>49</v>
       </c>
       <c r="D18" s="29">
-        <v>2858.52</v>
+        <v>4535.52</v>
       </c>
       <c r="E18" s="30">
         <v>0</v>
       </c>
       <c r="F18" s="31">
         <f t="shared" si="0"/>
-        <v>-2858.52</v>
+        <v>-4535.52</v>
       </c>
       <c r="G18" s="32" t="str">
         <f t="shared" si="1"/>
@@ -2833,14 +2902,14 @@
         <v>55</v>
       </c>
       <c r="D20" s="29">
-        <v>207352.2</v>
+        <v>306824.016</v>
       </c>
       <c r="E20" s="30">
         <v>0</v>
       </c>
       <c r="F20" s="31">
         <f t="shared" si="0"/>
-        <v>-207352.2</v>
+        <v>-306824.016</v>
       </c>
       <c r="G20" s="32" t="str">
         <f t="shared" si="1"/>
@@ -2885,14 +2954,14 @@
         <v>61</v>
       </c>
       <c r="D22" s="29">
-        <v>27306.79</v>
+        <v>29306.79</v>
       </c>
       <c r="E22" s="30">
         <v>0</v>
       </c>
       <c r="F22" s="31">
         <f t="shared" si="0"/>
-        <v>-27306.79</v>
+        <v>-29306.79</v>
       </c>
       <c r="G22" s="32" t="str">
         <f t="shared" si="1"/>
@@ -2911,14 +2980,14 @@
         <v>64</v>
       </c>
       <c r="D23" s="29">
-        <v>14285.880000000001</v>
+        <v>27585.88</v>
       </c>
       <c r="E23" s="30">
         <v>0</v>
       </c>
       <c r="F23" s="31">
         <f t="shared" si="0"/>
-        <v>-14285.880000000001</v>
+        <v>-27585.88</v>
       </c>
       <c r="G23" s="32" t="str">
         <f t="shared" si="1"/>
@@ -2963,14 +3032,14 @@
         <v>70</v>
       </c>
       <c r="D25" s="29">
-        <v>93786</v>
+        <v>125046.99999</v>
       </c>
       <c r="E25" s="30">
         <v>0</v>
       </c>
       <c r="F25" s="31">
         <f t="shared" si="0"/>
-        <v>-93786</v>
+        <v>-125046.99999</v>
       </c>
       <c r="G25" s="32" t="str">
         <f t="shared" si="1"/>
@@ -2989,14 +3058,14 @@
         <v>73</v>
       </c>
       <c r="D26" s="29">
-        <v>15934.79</v>
+        <v>22139.79</v>
       </c>
       <c r="E26" s="30">
         <v>0</v>
       </c>
       <c r="F26" s="31">
         <f t="shared" si="0"/>
-        <v>-15934.79</v>
+        <v>-22139.79</v>
       </c>
       <c r="G26" s="32" t="str">
         <f t="shared" si="1"/>
@@ -3015,14 +3084,14 @@
         <v>76</v>
       </c>
       <c r="D27" s="29">
-        <v>14645.29</v>
+        <v>21880.29</v>
       </c>
       <c r="E27" s="30">
         <v>0</v>
       </c>
       <c r="F27" s="31">
         <f t="shared" si="0"/>
-        <v>-14645.29</v>
+        <v>-21880.29</v>
       </c>
       <c r="G27" s="32" t="str">
         <f t="shared" si="1"/>
@@ -3093,14 +3162,14 @@
         <v>85</v>
       </c>
       <c r="D30" s="29">
-        <v>32.79</v>
+        <v>182.79</v>
       </c>
       <c r="E30" s="30">
         <v>0</v>
       </c>
       <c r="F30" s="31">
         <f t="shared" si="0"/>
-        <v>-32.79</v>
+        <v>-182.79</v>
       </c>
       <c r="G30" s="32" t="str">
         <f t="shared" si="1"/>
@@ -3119,14 +3188,14 @@
         <v>88</v>
       </c>
       <c r="D31" s="29">
-        <v>2583.56</v>
+        <v>3183.56</v>
       </c>
       <c r="E31" s="30">
         <v>0</v>
       </c>
       <c r="F31" s="31">
         <f t="shared" si="0"/>
-        <v>-2583.56</v>
+        <v>-3183.56</v>
       </c>
       <c r="G31" s="32" t="str">
         <f t="shared" si="1"/>
@@ -3145,14 +3214,14 @@
         <v>91</v>
       </c>
       <c r="D32" s="29">
-        <v>43192.35</v>
+        <v>57589.35</v>
       </c>
       <c r="E32" s="30">
         <v>0</v>
       </c>
       <c r="F32" s="31">
         <f t="shared" si="0"/>
-        <v>-43192.35</v>
+        <v>-57589.35</v>
       </c>
       <c r="G32" s="32" t="str">
         <f t="shared" si="1"/>
@@ -3171,14 +3240,14 @@
         <v>94</v>
       </c>
       <c r="D33" s="29">
-        <v>153638.28</v>
+        <v>204851.28</v>
       </c>
       <c r="E33" s="30">
         <v>0</v>
       </c>
       <c r="F33" s="31">
         <f t="shared" si="0"/>
-        <v>-153638.28</v>
+        <v>-204851.28</v>
       </c>
       <c r="G33" s="32" t="str">
         <f t="shared" si="1"/>
@@ -3197,14 +3266,14 @@
         <v>97</v>
       </c>
       <c r="D34" s="29">
-        <v>3743.89</v>
+        <v>5249.89</v>
       </c>
       <c r="E34" s="30">
         <v>0</v>
       </c>
       <c r="F34" s="31">
         <f t="shared" si="0"/>
-        <v>-3743.89</v>
+        <v>-5249.89</v>
       </c>
       <c r="G34" s="32" t="str">
         <f t="shared" si="1"/>
@@ -3223,14 +3292,14 @@
         <v>100</v>
       </c>
       <c r="D35" s="29">
-        <v>177558.31</v>
+        <v>220053.31</v>
       </c>
       <c r="E35" s="30">
         <v>0</v>
       </c>
       <c r="F35" s="31">
         <f t="shared" si="0"/>
-        <v>-177558.31</v>
+        <v>-220053.31</v>
       </c>
       <c r="G35" s="32" t="str">
         <f t="shared" si="1"/>
@@ -3249,14 +3318,14 @@
         <v>103</v>
       </c>
       <c r="D36" s="29">
-        <v>87713.05</v>
+        <v>116270.05</v>
       </c>
       <c r="E36" s="30">
         <v>0</v>
       </c>
       <c r="F36" s="31">
         <f t="shared" si="0"/>
-        <v>-87713.05</v>
+        <v>-116270.05</v>
       </c>
       <c r="G36" s="32" t="str">
         <f t="shared" si="1"/>
@@ -3275,14 +3344,14 @@
         <v>106</v>
       </c>
       <c r="D37" s="29">
-        <v>28637.55</v>
+        <v>38183.55</v>
       </c>
       <c r="E37" s="30">
         <v>0</v>
       </c>
       <c r="F37" s="31">
         <f t="shared" si="0"/>
-        <v>-28637.55</v>
+        <v>-38183.55</v>
       </c>
       <c r="G37" s="32" t="str">
         <f t="shared" si="1"/>
@@ -3353,14 +3422,14 @@
         <v>115</v>
       </c>
       <c r="D40" s="29">
-        <v>172642.96</v>
+        <v>265942.96</v>
       </c>
       <c r="E40" s="30">
         <v>0</v>
       </c>
       <c r="F40" s="31">
         <f t="shared" ref="F40:F71" si="2">E40-D40</f>
-        <v>-172642.96</v>
+        <v>-265942.96</v>
       </c>
       <c r="G40" s="32" t="str">
         <f t="shared" ref="G40:G71" si="3">IF(E40=0,"-",IF(D40=0,"*",F40/D40))</f>
@@ -3379,14 +3448,14 @@
         <v>118</v>
       </c>
       <c r="D41" s="29">
-        <v>66948.13</v>
+        <v>90383.13</v>
       </c>
       <c r="E41" s="30">
         <v>0</v>
       </c>
       <c r="F41" s="31">
         <f t="shared" si="2"/>
-        <v>-66948.13</v>
+        <v>-90383.13</v>
       </c>
       <c r="G41" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3405,14 +3474,14 @@
         <v>121</v>
       </c>
       <c r="D42" s="29">
-        <v>10171.07</v>
+        <v>17098.07</v>
       </c>
       <c r="E42" s="30">
         <v>0</v>
       </c>
       <c r="F42" s="31">
         <f t="shared" si="2"/>
-        <v>-10171.07</v>
+        <v>-17098.07</v>
       </c>
       <c r="G42" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3483,14 +3552,14 @@
         <v>130</v>
       </c>
       <c r="D45" s="29">
-        <v>94292.75</v>
+        <v>148292.75</v>
       </c>
       <c r="E45" s="30">
         <v>0</v>
       </c>
       <c r="F45" s="31">
         <f t="shared" si="2"/>
-        <v>-94292.75</v>
+        <v>-148292.75</v>
       </c>
       <c r="G45" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3509,14 +3578,14 @@
         <v>133</v>
       </c>
       <c r="D46" s="29">
-        <v>105669.85</v>
+        <v>168714.85</v>
       </c>
       <c r="E46" s="30">
         <v>0</v>
       </c>
       <c r="F46" s="31">
         <f t="shared" si="2"/>
-        <v>-105669.85</v>
+        <v>-168714.85</v>
       </c>
       <c r="G46" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3535,14 +3604,14 @@
         <v>136</v>
       </c>
       <c r="D47" s="29">
-        <v>98840.85</v>
+        <v>156440.85</v>
       </c>
       <c r="E47" s="30">
         <v>0</v>
       </c>
       <c r="F47" s="31">
         <f t="shared" si="2"/>
-        <v>-98840.85</v>
+        <v>-156440.85</v>
       </c>
       <c r="G47" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3587,14 +3656,14 @@
         <v>142</v>
       </c>
       <c r="D49" s="29">
-        <v>24300</v>
+        <v>39849</v>
       </c>
       <c r="E49" s="30">
         <v>0</v>
       </c>
       <c r="F49" s="31">
         <f t="shared" si="2"/>
-        <v>-24300</v>
+        <v>-39849</v>
       </c>
       <c r="G49" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3639,14 +3708,14 @@
         <v>148</v>
       </c>
       <c r="D51" s="29">
-        <v>1579.52</v>
+        <v>1000</v>
       </c>
       <c r="E51" s="30">
         <v>0</v>
       </c>
       <c r="F51" s="31">
         <f t="shared" si="2"/>
-        <v>-1579.52</v>
+        <v>-1000</v>
       </c>
       <c r="G51" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3665,14 +3734,14 @@
         <v>151</v>
       </c>
       <c r="D52" s="29">
-        <v>57485.880000000005</v>
+        <v>2639.66</v>
       </c>
       <c r="E52" s="30">
         <v>0</v>
       </c>
       <c r="F52" s="31">
         <f t="shared" si="2"/>
-        <v>-57485.880000000005</v>
+        <v>-2639.66</v>
       </c>
       <c r="G52" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3691,14 +3760,14 @@
         <v>154</v>
       </c>
       <c r="D53" s="29">
-        <v>7816</v>
+        <v>81729.90000000001</v>
       </c>
       <c r="E53" s="30">
         <v>0</v>
       </c>
       <c r="F53" s="31">
         <f t="shared" si="2"/>
-        <v>-7816</v>
+        <v>-81729.90000000001</v>
       </c>
       <c r="G53" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3717,14 +3786,14 @@
         <v>157</v>
       </c>
       <c r="D54" s="29">
-        <v>6146.6</v>
+        <v>11758</v>
       </c>
       <c r="E54" s="30">
         <v>0</v>
       </c>
       <c r="F54" s="31">
         <f t="shared" si="2"/>
-        <v>-6146.6</v>
+        <v>-11758</v>
       </c>
       <c r="G54" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3743,14 +3812,14 @@
         <v>160</v>
       </c>
       <c r="D55" s="29">
-        <v>980</v>
+        <v>8306.6</v>
       </c>
       <c r="E55" s="30">
         <v>0</v>
       </c>
       <c r="F55" s="31">
         <f t="shared" si="2"/>
-        <v>-980</v>
+        <v>-8306.6</v>
       </c>
       <c r="G55" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3769,14 +3838,14 @@
         <v>163</v>
       </c>
       <c r="D56" s="29">
-        <v>52296.46</v>
+        <v>980</v>
       </c>
       <c r="E56" s="30">
         <v>0</v>
       </c>
       <c r="F56" s="31">
         <f t="shared" si="2"/>
-        <v>-52296.46</v>
+        <v>-980</v>
       </c>
       <c r="G56" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3795,14 +3864,14 @@
         <v>166</v>
       </c>
       <c r="D57" s="29">
-        <v>1390.29</v>
+        <v>79296.46</v>
       </c>
       <c r="E57" s="30">
         <v>0</v>
       </c>
       <c r="F57" s="31">
         <f t="shared" si="2"/>
-        <v>-1390.29</v>
+        <v>-79296.46</v>
       </c>
       <c r="G57" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3821,14 +3890,14 @@
         <v>169</v>
       </c>
       <c r="D58" s="29">
-        <v>1492.04</v>
+        <v>1390.29</v>
       </c>
       <c r="E58" s="30">
         <v>0</v>
       </c>
       <c r="F58" s="31">
         <f t="shared" si="2"/>
-        <v>-1492.04</v>
+        <v>-1390.29</v>
       </c>
       <c r="G58" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3847,14 +3916,14 @@
         <v>172</v>
       </c>
       <c r="D59" s="29">
-        <v>5098.55</v>
+        <v>1492.04</v>
       </c>
       <c r="E59" s="30">
         <v>0</v>
       </c>
       <c r="F59" s="31">
         <f t="shared" si="2"/>
-        <v>-5098.55</v>
+        <v>-1492.04</v>
       </c>
       <c r="G59" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3873,14 +3942,14 @@
         <v>175</v>
       </c>
       <c r="D60" s="29">
-        <v>2727.2400000000002</v>
+        <v>5098.55</v>
       </c>
       <c r="E60" s="30">
         <v>0</v>
       </c>
       <c r="F60" s="31">
         <f t="shared" si="2"/>
-        <v>-2727.2400000000002</v>
+        <v>-5098.55</v>
       </c>
       <c r="G60" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3899,14 +3968,14 @@
         <v>178</v>
       </c>
       <c r="D61" s="29">
-        <v>48880</v>
+        <v>2727.2400000000002</v>
       </c>
       <c r="E61" s="30">
         <v>0</v>
       </c>
       <c r="F61" s="31">
         <f t="shared" si="2"/>
-        <v>-48880</v>
+        <v>-2727.2400000000002</v>
       </c>
       <c r="G61" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3925,14 +3994,14 @@
         <v>181</v>
       </c>
       <c r="D62" s="29">
-        <v>453</v>
+        <v>67380</v>
       </c>
       <c r="E62" s="30">
         <v>0</v>
       </c>
       <c r="F62" s="31">
         <f t="shared" si="2"/>
-        <v>-453</v>
+        <v>-67380</v>
       </c>
       <c r="G62" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3951,14 +4020,14 @@
         <v>184</v>
       </c>
       <c r="D63" s="29">
-        <v>3211.03</v>
+        <v>453</v>
       </c>
       <c r="E63" s="30">
         <v>0</v>
       </c>
       <c r="F63" s="31">
         <f t="shared" si="2"/>
-        <v>-3211.03</v>
+        <v>-453</v>
       </c>
       <c r="G63" s="32" t="str">
         <f t="shared" si="3"/>
@@ -3977,14 +4046,14 @@
         <v>187</v>
       </c>
       <c r="D64" s="29">
-        <v>2534.01</v>
+        <v>4011.03</v>
       </c>
       <c r="E64" s="30">
         <v>0</v>
       </c>
       <c r="F64" s="31">
         <f t="shared" si="2"/>
-        <v>-2534.01</v>
+        <v>-4011.03</v>
       </c>
       <c r="G64" s="32" t="str">
         <f t="shared" si="3"/>
@@ -4003,14 +4072,14 @@
         <v>190</v>
       </c>
       <c r="D65" s="29">
-        <v>941.16</v>
+        <v>4134.01</v>
       </c>
       <c r="E65" s="30">
         <v>0</v>
       </c>
       <c r="F65" s="31">
         <f t="shared" si="2"/>
-        <v>-941.16</v>
+        <v>-4134.01</v>
       </c>
       <c r="G65" s="32" t="str">
         <f t="shared" si="3"/>
@@ -4029,14 +4098,14 @@
         <v>193</v>
       </c>
       <c r="D66" s="29">
-        <v>675.0500000000001</v>
+        <v>1661.16</v>
       </c>
       <c r="E66" s="30">
         <v>0</v>
       </c>
       <c r="F66" s="31">
         <f t="shared" si="2"/>
-        <v>-675.0500000000001</v>
+        <v>-1661.16</v>
       </c>
       <c r="G66" s="32" t="str">
         <f t="shared" si="3"/>
@@ -4055,14 +4124,14 @@
         <v>196</v>
       </c>
       <c r="D67" s="29">
-        <v>384.48</v>
+        <v>2175.05</v>
       </c>
       <c r="E67" s="30">
         <v>0</v>
       </c>
       <c r="F67" s="31">
         <f t="shared" si="2"/>
-        <v>-384.48</v>
+        <v>-2175.05</v>
       </c>
       <c r="G67" s="32" t="str">
         <f t="shared" si="3"/>
@@ -4081,14 +4150,14 @@
         <v>199</v>
       </c>
       <c r="D68" s="29">
-        <v>105648.16</v>
+        <v>434.48</v>
       </c>
       <c r="E68" s="30">
         <v>0</v>
       </c>
       <c r="F68" s="31">
         <f t="shared" si="2"/>
-        <v>-105648.16</v>
+        <v>-434.48</v>
       </c>
       <c r="G68" s="32" t="str">
         <f t="shared" si="3"/>
@@ -4107,14 +4176,14 @@
         <v>202</v>
       </c>
       <c r="D69" s="29">
-        <v>19854.74</v>
+        <v>165333.16</v>
       </c>
       <c r="E69" s="30">
         <v>0</v>
       </c>
       <c r="F69" s="31">
         <f t="shared" si="2"/>
-        <v>-19854.74</v>
+        <v>-165333.16</v>
       </c>
       <c r="G69" s="32" t="str">
         <f t="shared" si="3"/>
@@ -4133,14 +4202,14 @@
         <v>205</v>
       </c>
       <c r="D70" s="29">
-        <v>100.65</v>
+        <v>27522.74</v>
       </c>
       <c r="E70" s="30">
         <v>0</v>
       </c>
       <c r="F70" s="31">
         <f t="shared" si="2"/>
-        <v>-100.65</v>
+        <v>-27522.74</v>
       </c>
       <c r="G70" s="32" t="str">
         <f t="shared" si="3"/>
@@ -4159,14 +4228,14 @@
         <v>208</v>
       </c>
       <c r="D71" s="29">
-        <v>18</v>
+        <v>151.65</v>
       </c>
       <c r="E71" s="30">
         <v>0</v>
       </c>
       <c r="F71" s="31">
         <f t="shared" si="2"/>
-        <v>-18</v>
+        <v>-151.65</v>
       </c>
       <c r="G71" s="32" t="str">
         <f t="shared" si="3"/>
@@ -4185,14 +4254,14 @@
         <v>211</v>
       </c>
       <c r="D72" s="29">
-        <v>-18</v>
+        <v>18</v>
       </c>
       <c r="E72" s="30">
         <v>0</v>
       </c>
       <c r="F72" s="31">
         <f t="shared" ref="F72:F103" si="4">E72-D72</f>
-        <v>18</v>
+        <v>-18</v>
       </c>
       <c r="G72" s="32" t="str">
         <f t="shared" ref="G72:G103" si="5">IF(E72=0,"-",IF(D72=0,"*",F72/D72))</f>
@@ -4211,14 +4280,14 @@
         <v>214</v>
       </c>
       <c r="D73" s="29">
-        <v>13839.36</v>
+        <v>-18</v>
       </c>
       <c r="E73" s="30">
         <v>0</v>
       </c>
       <c r="F73" s="31">
         <f t="shared" si="4"/>
-        <v>-13839.36</v>
+        <v>18</v>
       </c>
       <c r="G73" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4237,14 +4306,14 @@
         <v>217</v>
       </c>
       <c r="D74" s="29">
-        <v>50982.17</v>
+        <v>20829.36</v>
       </c>
       <c r="E74" s="30">
         <v>0</v>
       </c>
       <c r="F74" s="31">
         <f t="shared" si="4"/>
-        <v>-50982.17</v>
+        <v>-20829.36</v>
       </c>
       <c r="G74" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4263,14 +4332,14 @@
         <v>220</v>
       </c>
       <c r="D75" s="29">
-        <v>11036</v>
+        <v>70377.17</v>
       </c>
       <c r="E75" s="30">
         <v>0</v>
       </c>
       <c r="F75" s="31">
         <f t="shared" si="4"/>
-        <v>-11036</v>
+        <v>-70377.17</v>
       </c>
       <c r="G75" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4289,14 +4358,14 @@
         <v>223</v>
       </c>
       <c r="D76" s="29">
-        <v>5154.88</v>
+        <v>20759</v>
       </c>
       <c r="E76" s="30">
         <v>0</v>
       </c>
       <c r="F76" s="31">
         <f t="shared" si="4"/>
-        <v>-5154.88</v>
+        <v>-20759</v>
       </c>
       <c r="G76" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4315,14 +4384,14 @@
         <v>226</v>
       </c>
       <c r="D77" s="29">
-        <v>654.15</v>
+        <v>8294.880000000001</v>
       </c>
       <c r="E77" s="30">
         <v>0</v>
       </c>
       <c r="F77" s="31">
         <f t="shared" si="4"/>
-        <v>-654.15</v>
+        <v>-8294.880000000001</v>
       </c>
       <c r="G77" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4341,14 +4410,14 @@
         <v>229</v>
       </c>
       <c r="D78" s="29">
-        <v>15138.78</v>
+        <v>983.4</v>
       </c>
       <c r="E78" s="30">
         <v>0</v>
       </c>
       <c r="F78" s="31">
         <f t="shared" si="4"/>
-        <v>-15138.78</v>
+        <v>-983.4</v>
       </c>
       <c r="G78" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4367,14 +4436,14 @@
         <v>232</v>
       </c>
       <c r="D79" s="29">
-        <v>6089.650000000001</v>
+        <v>22167.510000000002</v>
       </c>
       <c r="E79" s="30">
         <v>0</v>
       </c>
       <c r="F79" s="31">
         <f t="shared" si="4"/>
-        <v>-6089.650000000001</v>
+        <v>-22167.510000000002</v>
       </c>
       <c r="G79" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4393,14 +4462,14 @@
         <v>235</v>
       </c>
       <c r="D80" s="29">
-        <v>4505.78</v>
+        <v>6089.650000000001</v>
       </c>
       <c r="E80" s="30">
         <v>0</v>
       </c>
       <c r="F80" s="31">
         <f t="shared" si="4"/>
-        <v>-4505.78</v>
+        <v>-6089.650000000001</v>
       </c>
       <c r="G80" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4419,14 +4488,14 @@
         <v>238</v>
       </c>
       <c r="D81" s="29">
-        <v>270.92</v>
+        <v>6182.78</v>
       </c>
       <c r="E81" s="30">
         <v>0</v>
       </c>
       <c r="F81" s="31">
         <f t="shared" si="4"/>
-        <v>-270.92</v>
+        <v>-6182.78</v>
       </c>
       <c r="G81" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4445,14 +4514,14 @@
         <v>241</v>
       </c>
       <c r="D82" s="29">
-        <v>1750.55</v>
+        <v>270.92</v>
       </c>
       <c r="E82" s="30">
         <v>0</v>
       </c>
       <c r="F82" s="31">
         <f t="shared" si="4"/>
-        <v>-1750.55</v>
+        <v>-270.92</v>
       </c>
       <c r="G82" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4471,14 +4540,14 @@
         <v>244</v>
       </c>
       <c r="D83" s="29">
-        <v>490</v>
+        <v>1750.55</v>
       </c>
       <c r="E83" s="30">
         <v>0</v>
       </c>
       <c r="F83" s="31">
         <f t="shared" si="4"/>
-        <v>-490</v>
+        <v>-1750.55</v>
       </c>
       <c r="G83" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4497,14 +4566,14 @@
         <v>247</v>
       </c>
       <c r="D84" s="29">
-        <v>325.38</v>
+        <v>490</v>
       </c>
       <c r="E84" s="30">
         <v>0</v>
       </c>
       <c r="F84" s="31">
         <f t="shared" si="4"/>
-        <v>-325.38</v>
+        <v>-490</v>
       </c>
       <c r="G84" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4523,14 +4592,14 @@
         <v>250</v>
       </c>
       <c r="D85" s="29">
-        <v>8367.3</v>
+        <v>1325.38</v>
       </c>
       <c r="E85" s="30">
         <v>0</v>
       </c>
       <c r="F85" s="31">
         <f t="shared" si="4"/>
-        <v>-8367.3</v>
+        <v>-1325.38</v>
       </c>
       <c r="G85" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4549,14 +4618,14 @@
         <v>253</v>
       </c>
       <c r="D86" s="29">
-        <v>282</v>
+        <v>11157.300000000001</v>
       </c>
       <c r="E86" s="30">
         <v>0</v>
       </c>
       <c r="F86" s="31">
         <f t="shared" si="4"/>
-        <v>-282</v>
+        <v>-11157.300000000001</v>
       </c>
       <c r="G86" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4575,14 +4644,14 @@
         <v>256</v>
       </c>
       <c r="D87" s="29">
-        <v>5982</v>
+        <v>372</v>
       </c>
       <c r="E87" s="30">
         <v>0</v>
       </c>
       <c r="F87" s="31">
         <f t="shared" si="4"/>
-        <v>-5982</v>
+        <v>-372</v>
       </c>
       <c r="G87" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4601,14 +4670,14 @@
         <v>259</v>
       </c>
       <c r="D88" s="29">
-        <v>1215</v>
+        <v>6957</v>
       </c>
       <c r="E88" s="30">
         <v>0</v>
       </c>
       <c r="F88" s="31">
         <f t="shared" si="4"/>
-        <v>-1215</v>
+        <v>-6957</v>
       </c>
       <c r="G88" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4627,14 +4696,14 @@
         <v>262</v>
       </c>
       <c r="D89" s="29">
-        <v>260.38</v>
+        <v>2061</v>
       </c>
       <c r="E89" s="30">
         <v>0</v>
       </c>
       <c r="F89" s="31">
         <f t="shared" si="4"/>
-        <v>-260.38</v>
+        <v>-2061</v>
       </c>
       <c r="G89" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4653,14 +4722,14 @@
         <v>265</v>
       </c>
       <c r="D90" s="29">
-        <v>1195.89</v>
+        <v>360.38</v>
       </c>
       <c r="E90" s="30">
         <v>0</v>
       </c>
       <c r="F90" s="31">
         <f t="shared" si="4"/>
-        <v>-1195.89</v>
+        <v>-360.38</v>
       </c>
       <c r="G90" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4679,14 +4748,14 @@
         <v>268</v>
       </c>
       <c r="D91" s="29">
-        <v>214674.17</v>
+        <v>1435.89</v>
       </c>
       <c r="E91" s="30">
         <v>0</v>
       </c>
       <c r="F91" s="31">
         <f t="shared" si="4"/>
-        <v>-214674.17</v>
+        <v>-1435.89</v>
       </c>
       <c r="G91" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4705,14 +4774,14 @@
         <v>271</v>
       </c>
       <c r="D92" s="29">
-        <v>1796.6200000000001</v>
+        <v>317247.17</v>
       </c>
       <c r="E92" s="30">
         <v>0</v>
       </c>
       <c r="F92" s="31">
         <f t="shared" si="4"/>
-        <v>-1796.6200000000001</v>
+        <v>-317247.17</v>
       </c>
       <c r="G92" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4731,14 +4800,14 @@
         <v>274</v>
       </c>
       <c r="D93" s="29">
-        <v>10867.56</v>
+        <v>28196.62</v>
       </c>
       <c r="E93" s="30">
         <v>0</v>
       </c>
       <c r="F93" s="31">
         <f t="shared" si="4"/>
-        <v>-10867.56</v>
+        <v>-28196.62</v>
       </c>
       <c r="G93" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4757,14 +4826,14 @@
         <v>277</v>
       </c>
       <c r="D94" s="29">
-        <v>10157.28</v>
+        <v>16267.56</v>
       </c>
       <c r="E94" s="30">
         <v>0</v>
       </c>
       <c r="F94" s="31">
         <f t="shared" si="4"/>
-        <v>-10157.28</v>
+        <v>-16267.56</v>
       </c>
       <c r="G94" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4783,14 +4852,14 @@
         <v>280</v>
       </c>
       <c r="D95" s="29">
-        <v>-3156.56</v>
+        <v>10157.28</v>
       </c>
       <c r="E95" s="30">
         <v>0</v>
       </c>
       <c r="F95" s="31">
         <f t="shared" si="4"/>
-        <v>3156.56</v>
+        <v>-10157.28</v>
       </c>
       <c r="G95" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4809,14 +4878,14 @@
         <v>283</v>
       </c>
       <c r="D96" s="29">
-        <v>2074.94</v>
+        <v>-3156.56</v>
       </c>
       <c r="E96" s="30">
         <v>0</v>
       </c>
       <c r="F96" s="31">
         <f t="shared" si="4"/>
-        <v>-2074.94</v>
+        <v>3156.56</v>
       </c>
       <c r="G96" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4835,14 +4904,14 @@
         <v>286</v>
       </c>
       <c r="D97" s="29">
-        <v>34156.44</v>
+        <v>2782.94</v>
       </c>
       <c r="E97" s="30">
         <v>0</v>
       </c>
       <c r="F97" s="31">
         <f t="shared" si="4"/>
-        <v>-34156.44</v>
+        <v>-2782.94</v>
       </c>
       <c r="G97" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4861,14 +4930,14 @@
         <v>289</v>
       </c>
       <c r="D98" s="29">
-        <v>18447</v>
+        <v>46003.44</v>
       </c>
       <c r="E98" s="30">
         <v>0</v>
       </c>
       <c r="F98" s="31">
         <f t="shared" si="4"/>
-        <v>-18447</v>
+        <v>-46003.44</v>
       </c>
       <c r="G98" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4887,14 +4956,14 @@
         <v>292</v>
       </c>
       <c r="D99" s="29">
-        <v>8985.57</v>
+        <v>31443</v>
       </c>
       <c r="E99" s="30">
         <v>0</v>
       </c>
       <c r="F99" s="31">
         <f t="shared" si="4"/>
-        <v>-8985.57</v>
+        <v>-31443</v>
       </c>
       <c r="G99" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4913,14 +4982,14 @@
         <v>295</v>
       </c>
       <c r="D100" s="29">
-        <v>15583.68</v>
+        <v>35982.57</v>
       </c>
       <c r="E100" s="30">
         <v>0</v>
       </c>
       <c r="F100" s="31">
         <f t="shared" si="4"/>
-        <v>-15583.68</v>
+        <v>-35982.57</v>
       </c>
       <c r="G100" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4939,14 +5008,14 @@
         <v>298</v>
       </c>
       <c r="D101" s="29">
-        <v>5314.32</v>
+        <v>20782.68</v>
       </c>
       <c r="E101" s="30">
         <v>0</v>
       </c>
       <c r="F101" s="31">
         <f t="shared" si="4"/>
-        <v>-5314.32</v>
+        <v>-20782.68</v>
       </c>
       <c r="G101" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4965,14 +5034,14 @@
         <v>301</v>
       </c>
       <c r="D102" s="29">
-        <v>2299</v>
+        <v>7304.32</v>
       </c>
       <c r="E102" s="30">
         <v>0</v>
       </c>
       <c r="F102" s="31">
         <f t="shared" si="4"/>
-        <v>-2299</v>
+        <v>-7304.32</v>
       </c>
       <c r="G102" s="32" t="str">
         <f t="shared" si="5"/>
@@ -4991,14 +5060,14 @@
         <v>304</v>
       </c>
       <c r="D103" s="29">
-        <v>286.16</v>
+        <v>2299</v>
       </c>
       <c r="E103" s="30">
         <v>0</v>
       </c>
       <c r="F103" s="31">
         <f t="shared" si="4"/>
-        <v>-286.16</v>
+        <v>-2299</v>
       </c>
       <c r="G103" s="32" t="str">
         <f t="shared" si="5"/>
@@ -5017,14 +5086,14 @@
         <v>307</v>
       </c>
       <c r="D104" s="29">
-        <v>177.96</v>
+        <v>886.16</v>
       </c>
       <c r="E104" s="30">
         <v>0</v>
       </c>
       <c r="F104" s="31">
         <f t="shared" ref="F104:F135" si="6">E104-D104</f>
-        <v>-177.96</v>
+        <v>-886.16</v>
       </c>
       <c r="G104" s="32" t="str">
         <f t="shared" ref="G104:G135" si="7">IF(E104=0,"-",IF(D104=0,"*",F104/D104))</f>
@@ -5043,14 +5112,14 @@
         <v>310</v>
       </c>
       <c r="D105" s="29">
-        <v>1928.75</v>
+        <v>2677.96</v>
       </c>
       <c r="E105" s="30">
         <v>0</v>
       </c>
       <c r="F105" s="31">
         <f t="shared" si="6"/>
-        <v>-1928.75</v>
+        <v>-2677.96</v>
       </c>
       <c r="G105" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5069,14 +5138,14 @@
         <v>313</v>
       </c>
       <c r="D106" s="29">
-        <v>360</v>
+        <v>2828.75</v>
       </c>
       <c r="E106" s="30">
         <v>0</v>
       </c>
       <c r="F106" s="31">
         <f t="shared" si="6"/>
-        <v>-360</v>
+        <v>-2828.75</v>
       </c>
       <c r="G106" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5095,14 +5164,14 @@
         <v>316</v>
       </c>
       <c r="D107" s="29">
-        <v>3727.61</v>
+        <v>840</v>
       </c>
       <c r="E107" s="30">
         <v>0</v>
       </c>
       <c r="F107" s="31">
         <f t="shared" si="6"/>
-        <v>-3727.61</v>
+        <v>-840</v>
       </c>
       <c r="G107" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5121,14 +5190,14 @@
         <v>319</v>
       </c>
       <c r="D108" s="29">
-        <v>2615.83</v>
+        <v>150</v>
       </c>
       <c r="E108" s="30">
         <v>0</v>
       </c>
       <c r="F108" s="31">
         <f t="shared" si="6"/>
-        <v>-2615.83</v>
+        <v>-150</v>
       </c>
       <c r="G108" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5147,14 +5216,14 @@
         <v>322</v>
       </c>
       <c r="D109" s="29">
-        <v>836</v>
+        <v>7267.610000000001</v>
       </c>
       <c r="E109" s="30">
         <v>0</v>
       </c>
       <c r="F109" s="31">
         <f t="shared" si="6"/>
-        <v>-836</v>
+        <v>-7267.610000000001</v>
       </c>
       <c r="G109" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5173,14 +5242,14 @@
         <v>325</v>
       </c>
       <c r="D110" s="29">
-        <v>2786.3</v>
+        <v>4145.83</v>
       </c>
       <c r="E110" s="30">
         <v>0</v>
       </c>
       <c r="F110" s="31">
         <f t="shared" si="6"/>
-        <v>-2786.3</v>
+        <v>-4145.83</v>
       </c>
       <c r="G110" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5199,14 +5268,14 @@
         <v>328</v>
       </c>
       <c r="D111" s="29">
-        <v>487.5</v>
+        <v>1496</v>
       </c>
       <c r="E111" s="30">
         <v>0</v>
       </c>
       <c r="F111" s="31">
         <f t="shared" si="6"/>
-        <v>-487.5</v>
+        <v>-1496</v>
       </c>
       <c r="G111" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5225,14 +5294,14 @@
         <v>331</v>
       </c>
       <c r="D112" s="29">
-        <v>11534.25</v>
+        <v>4700.3</v>
       </c>
       <c r="E112" s="30">
         <v>0</v>
       </c>
       <c r="F112" s="31">
         <f t="shared" si="6"/>
-        <v>-11534.25</v>
+        <v>-4700.3</v>
       </c>
       <c r="G112" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5251,14 +5320,14 @@
         <v>334</v>
       </c>
       <c r="D113" s="29">
-        <v>4455</v>
+        <v>832.5</v>
       </c>
       <c r="E113" s="30">
         <v>0</v>
       </c>
       <c r="F113" s="31">
         <f t="shared" si="6"/>
-        <v>-4455</v>
+        <v>-832.5</v>
       </c>
       <c r="G113" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5277,14 +5346,14 @@
         <v>337</v>
       </c>
       <c r="D114" s="29">
-        <v>6893.87</v>
+        <v>15734.25</v>
       </c>
       <c r="E114" s="30">
         <v>0</v>
       </c>
       <c r="F114" s="31">
         <f t="shared" si="6"/>
-        <v>-6893.87</v>
+        <v>-15734.25</v>
       </c>
       <c r="G114" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5303,14 +5372,14 @@
         <v>340</v>
       </c>
       <c r="D115" s="29">
-        <v>998</v>
+        <v>5955</v>
       </c>
       <c r="E115" s="30">
         <v>0</v>
       </c>
       <c r="F115" s="31">
         <f t="shared" si="6"/>
-        <v>-998</v>
+        <v>-5955</v>
       </c>
       <c r="G115" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5329,14 +5398,14 @@
         <v>343</v>
       </c>
       <c r="D116" s="29">
-        <v>28340.58</v>
+        <v>300</v>
       </c>
       <c r="E116" s="30">
         <v>0</v>
       </c>
       <c r="F116" s="31">
         <f t="shared" si="6"/>
-        <v>-28340.58</v>
+        <v>-300</v>
       </c>
       <c r="G116" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5355,14 +5424,14 @@
         <v>346</v>
       </c>
       <c r="D117" s="29">
-        <v>154.35</v>
+        <v>9143.87</v>
       </c>
       <c r="E117" s="30">
         <v>0</v>
       </c>
       <c r="F117" s="31">
         <f t="shared" si="6"/>
-        <v>-154.35</v>
+        <v>-9143.87</v>
       </c>
       <c r="G117" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5381,14 +5450,14 @@
         <v>349</v>
       </c>
       <c r="D118" s="29">
-        <v>10011.9</v>
+        <v>2498</v>
       </c>
       <c r="E118" s="30">
         <v>0</v>
       </c>
       <c r="F118" s="31">
         <f t="shared" si="6"/>
-        <v>-10011.9</v>
+        <v>-2498</v>
       </c>
       <c r="G118" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5407,14 +5476,14 @@
         <v>352</v>
       </c>
       <c r="D119" s="29">
-        <v>36777.38</v>
+        <v>1500</v>
       </c>
       <c r="E119" s="30">
         <v>0</v>
       </c>
       <c r="F119" s="31">
         <f t="shared" si="6"/>
-        <v>-36777.38</v>
+        <v>-1500</v>
       </c>
       <c r="G119" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5433,14 +5502,14 @@
         <v>355</v>
       </c>
       <c r="D120" s="29">
-        <v>1290.24</v>
+        <v>37440.58</v>
       </c>
       <c r="E120" s="30">
         <v>0</v>
       </c>
       <c r="F120" s="31">
         <f t="shared" si="6"/>
-        <v>-1290.24</v>
+        <v>-37440.58</v>
       </c>
       <c r="G120" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5459,14 +5528,14 @@
         <v>358</v>
       </c>
       <c r="D121" s="29">
-        <v>35700.43</v>
+        <v>274.35</v>
       </c>
       <c r="E121" s="30">
         <v>0</v>
       </c>
       <c r="F121" s="31">
         <f t="shared" si="6"/>
-        <v>-35700.43</v>
+        <v>-274.35</v>
       </c>
       <c r="G121" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5485,14 +5554,14 @@
         <v>361</v>
       </c>
       <c r="D122" s="29">
-        <v>41006.090000000004</v>
+        <v>10011.9</v>
       </c>
       <c r="E122" s="30">
         <v>0</v>
       </c>
       <c r="F122" s="31">
         <f t="shared" si="6"/>
-        <v>-41006.090000000004</v>
+        <v>-10011.9</v>
       </c>
       <c r="G122" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5511,14 +5580,14 @@
         <v>364</v>
       </c>
       <c r="D123" s="29">
-        <v>26804.25</v>
+        <v>36777.38</v>
       </c>
       <c r="E123" s="30">
         <v>0</v>
       </c>
       <c r="F123" s="31">
         <f t="shared" si="6"/>
-        <v>-26804.25</v>
+        <v>-36777.38</v>
       </c>
       <c r="G123" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5537,14 +5606,14 @@
         <v>367</v>
       </c>
       <c r="D124" s="29">
-        <v>-140.48</v>
+        <v>1834.41</v>
       </c>
       <c r="E124" s="30">
         <v>0</v>
       </c>
       <c r="F124" s="31">
         <f t="shared" si="6"/>
-        <v>140.48</v>
+        <v>-1834.41</v>
       </c>
       <c r="G124" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5563,14 +5632,14 @@
         <v>370</v>
       </c>
       <c r="D125" s="29">
-        <v>108.34</v>
+        <v>35700.43</v>
       </c>
       <c r="E125" s="30">
         <v>0</v>
       </c>
       <c r="F125" s="31">
         <f t="shared" si="6"/>
-        <v>-108.34</v>
+        <v>-35700.43</v>
       </c>
       <c r="G125" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5589,14 +5658,14 @@
         <v>373</v>
       </c>
       <c r="D126" s="29">
-        <v>444.88</v>
+        <v>59332.19</v>
       </c>
       <c r="E126" s="30">
         <v>0</v>
       </c>
       <c r="F126" s="31">
         <f t="shared" si="6"/>
-        <v>-444.88</v>
+        <v>-59332.19</v>
       </c>
       <c r="G126" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5615,14 +5684,14 @@
         <v>376</v>
       </c>
       <c r="D127" s="29">
-        <v>-500</v>
+        <v>26804.25</v>
       </c>
       <c r="E127" s="30">
         <v>0</v>
       </c>
       <c r="F127" s="31">
         <f t="shared" si="6"/>
-        <v>500</v>
+        <v>-26804.25</v>
       </c>
       <c r="G127" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5641,14 +5710,14 @@
         <v>379</v>
       </c>
       <c r="D128" s="29">
-        <v>2405</v>
+        <v>-140.48</v>
       </c>
       <c r="E128" s="30">
         <v>0</v>
       </c>
       <c r="F128" s="31">
         <f t="shared" si="6"/>
-        <v>-2405</v>
+        <v>140.48</v>
       </c>
       <c r="G128" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5667,14 +5736,14 @@
         <v>382</v>
       </c>
       <c r="D129" s="29">
-        <v>186611.26</v>
+        <v>2008.3400000000001</v>
       </c>
       <c r="E129" s="30">
         <v>0</v>
       </c>
       <c r="F129" s="31">
         <f t="shared" si="6"/>
-        <v>-186611.26</v>
+        <v>-2008.3400000000001</v>
       </c>
       <c r="G129" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5693,14 +5762,14 @@
         <v>385</v>
       </c>
       <c r="D130" s="29">
-        <v>800</v>
+        <v>1444.88</v>
       </c>
       <c r="E130" s="30">
         <v>0</v>
       </c>
       <c r="F130" s="31">
         <f t="shared" si="6"/>
-        <v>-800</v>
+        <v>-1444.88</v>
       </c>
       <c r="G130" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5719,14 +5788,14 @@
         <v>388</v>
       </c>
       <c r="D131" s="29">
-        <v>435.34000000000003</v>
+        <v>-500</v>
       </c>
       <c r="E131" s="30">
         <v>0</v>
       </c>
       <c r="F131" s="31">
         <f t="shared" si="6"/>
-        <v>-435.34000000000003</v>
+        <v>500</v>
       </c>
       <c r="G131" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5745,14 +5814,14 @@
         <v>391</v>
       </c>
       <c r="D132" s="29">
-        <v>630</v>
+        <v>2405</v>
       </c>
       <c r="E132" s="30">
         <v>0</v>
       </c>
       <c r="F132" s="31">
         <f t="shared" si="6"/>
-        <v>-630</v>
+        <v>-2405</v>
       </c>
       <c r="G132" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5771,14 +5840,14 @@
         <v>394</v>
       </c>
       <c r="D133" s="29">
-        <v>8827.300000000001</v>
+        <v>186611.26</v>
       </c>
       <c r="E133" s="30">
         <v>0</v>
       </c>
       <c r="F133" s="31">
         <f t="shared" si="6"/>
-        <v>-8827.300000000001</v>
+        <v>-186611.26</v>
       </c>
       <c r="G133" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5797,14 +5866,14 @@
         <v>397</v>
       </c>
       <c r="D134" s="29">
-        <v>4475</v>
+        <v>800</v>
       </c>
       <c r="E134" s="30">
         <v>0</v>
       </c>
       <c r="F134" s="31">
         <f t="shared" si="6"/>
-        <v>-4475</v>
+        <v>-800</v>
       </c>
       <c r="G134" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5823,14 +5892,14 @@
         <v>400</v>
       </c>
       <c r="D135" s="29">
-        <v>623.3000000000001</v>
+        <v>3435.34</v>
       </c>
       <c r="E135" s="30">
         <v>0</v>
       </c>
       <c r="F135" s="31">
         <f t="shared" si="6"/>
-        <v>-623.3000000000001</v>
+        <v>-3435.34</v>
       </c>
       <c r="G135" s="32" t="str">
         <f t="shared" si="7"/>
@@ -5849,17 +5918,17 @@
         <v>403</v>
       </c>
       <c r="D136" s="29">
-        <v>1200</v>
+        <v>100</v>
       </c>
       <c r="E136" s="30">
         <v>0</v>
       </c>
       <c r="F136" s="31">
-        <f t="shared" ref="F136:F160" si="8">E136-D136</f>
-        <v>-1200</v>
+        <f t="shared" ref="F136:F167" si="8">E136-D136</f>
+        <v>-100</v>
       </c>
       <c r="G136" s="32" t="str">
-        <f t="shared" ref="G136:G161" si="9">IF(E136=0,"-",IF(D136=0,"*",F136/D136))</f>
+        <f t="shared" ref="G136:G167" si="9">IF(E136=0,"-",IF(D136=0,"*",F136/D136))</f>
         <v>-</v>
       </c>
       <c r="H136" s="33"/>
@@ -5875,14 +5944,14 @@
         <v>406</v>
       </c>
       <c r="D137" s="29">
-        <v>1626.66</v>
+        <v>630</v>
       </c>
       <c r="E137" s="30">
         <v>0</v>
       </c>
       <c r="F137" s="31">
         <f t="shared" si="8"/>
-        <v>-1626.66</v>
+        <v>-630</v>
       </c>
       <c r="G137" s="32" t="str">
         <f t="shared" si="9"/>
@@ -5901,14 +5970,14 @@
         <v>409</v>
       </c>
       <c r="D138" s="29">
-        <v>709.08</v>
+        <v>12352.300000000001</v>
       </c>
       <c r="E138" s="30">
         <v>0</v>
       </c>
       <c r="F138" s="31">
         <f t="shared" si="8"/>
-        <v>-709.08</v>
+        <v>-12352.300000000001</v>
       </c>
       <c r="G138" s="32" t="str">
         <f t="shared" si="9"/>
@@ -5927,14 +5996,14 @@
         <v>412</v>
       </c>
       <c r="D139" s="29">
-        <v>21078.66</v>
+        <v>4475</v>
       </c>
       <c r="E139" s="30">
         <v>0</v>
       </c>
       <c r="F139" s="31">
         <f t="shared" si="8"/>
-        <v>-21078.66</v>
+        <v>-4475</v>
       </c>
       <c r="G139" s="32" t="str">
         <f t="shared" si="9"/>
@@ -5953,14 +6022,14 @@
         <v>415</v>
       </c>
       <c r="D140" s="29">
-        <v>15058.5</v>
+        <v>623.3000000000001</v>
       </c>
       <c r="E140" s="30">
         <v>0</v>
       </c>
       <c r="F140" s="31">
         <f t="shared" si="8"/>
-        <v>-15058.5</v>
+        <v>-623.3000000000001</v>
       </c>
       <c r="G140" s="32" t="str">
         <f t="shared" si="9"/>
@@ -5979,14 +6048,14 @@
         <v>418</v>
       </c>
       <c r="D141" s="29">
-        <v>3983.2400000000002</v>
+        <v>1200</v>
       </c>
       <c r="E141" s="30">
         <v>0</v>
       </c>
       <c r="F141" s="31">
         <f t="shared" si="8"/>
-        <v>-3983.2400000000002</v>
+        <v>-1200</v>
       </c>
       <c r="G141" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6005,14 +6074,14 @@
         <v>421</v>
       </c>
       <c r="D142" s="29">
-        <v>5990.63</v>
+        <v>1626.66</v>
       </c>
       <c r="E142" s="30">
         <v>0</v>
       </c>
       <c r="F142" s="31">
         <f t="shared" si="8"/>
-        <v>-5990.63</v>
+        <v>-1626.66</v>
       </c>
       <c r="G142" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6031,14 +6100,14 @@
         <v>424</v>
       </c>
       <c r="D143" s="29">
-        <v>396.67</v>
+        <v>709.08</v>
       </c>
       <c r="E143" s="30">
         <v>0</v>
       </c>
       <c r="F143" s="31">
         <f t="shared" si="8"/>
-        <v>-396.67</v>
+        <v>-709.08</v>
       </c>
       <c r="G143" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6057,14 +6126,14 @@
         <v>427</v>
       </c>
       <c r="D144" s="29">
-        <v>524.34</v>
+        <v>21778.66</v>
       </c>
       <c r="E144" s="30">
         <v>0</v>
       </c>
       <c r="F144" s="31">
         <f t="shared" si="8"/>
-        <v>-524.34</v>
+        <v>-21778.66</v>
       </c>
       <c r="G144" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6083,14 +6152,14 @@
         <v>430</v>
       </c>
       <c r="D145" s="29">
-        <v>285.05</v>
+        <v>22558.5</v>
       </c>
       <c r="E145" s="30">
         <v>0</v>
       </c>
       <c r="F145" s="31">
         <f t="shared" si="8"/>
-        <v>-285.05</v>
+        <v>-22558.5</v>
       </c>
       <c r="G145" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6109,14 +6178,14 @@
         <v>433</v>
       </c>
       <c r="D146" s="29">
-        <v>759</v>
+        <v>4883.24</v>
       </c>
       <c r="E146" s="30">
         <v>0</v>
       </c>
       <c r="F146" s="31">
         <f t="shared" si="8"/>
-        <v>-759</v>
+        <v>-4883.24</v>
       </c>
       <c r="G146" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6135,14 +6204,14 @@
         <v>436</v>
       </c>
       <c r="D147" s="29">
-        <v>344.17</v>
+        <v>8390.630000000001</v>
       </c>
       <c r="E147" s="30">
         <v>0</v>
       </c>
       <c r="F147" s="31">
         <f t="shared" si="8"/>
-        <v>-344.17</v>
+        <v>-8390.630000000001</v>
       </c>
       <c r="G147" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6161,14 +6230,14 @@
         <v>439</v>
       </c>
       <c r="D148" s="29">
-        <v>14.26</v>
+        <v>396.67</v>
       </c>
       <c r="E148" s="30">
         <v>0</v>
       </c>
       <c r="F148" s="31">
         <f t="shared" si="8"/>
-        <v>-14.26</v>
+        <v>-396.67</v>
       </c>
       <c r="G148" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6187,14 +6256,14 @@
         <v>442</v>
       </c>
       <c r="D149" s="29">
-        <v>11062.49</v>
+        <v>524.34</v>
       </c>
       <c r="E149" s="30">
         <v>0</v>
       </c>
       <c r="F149" s="31">
         <f t="shared" si="8"/>
-        <v>-11062.49</v>
+        <v>-524.34</v>
       </c>
       <c r="G149" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6213,14 +6282,14 @@
         <v>445</v>
       </c>
       <c r="D150" s="29">
-        <v>30296.12</v>
+        <v>485.05</v>
       </c>
       <c r="E150" s="30">
         <v>0</v>
       </c>
       <c r="F150" s="31">
         <f t="shared" si="8"/>
-        <v>-30296.12</v>
+        <v>-485.05</v>
       </c>
       <c r="G150" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6239,14 +6308,14 @@
         <v>448</v>
       </c>
       <c r="D151" s="29">
-        <v>8154.68</v>
+        <v>1159</v>
       </c>
       <c r="E151" s="30">
         <v>0</v>
       </c>
       <c r="F151" s="31">
         <f t="shared" si="8"/>
-        <v>-8154.68</v>
+        <v>-1159</v>
       </c>
       <c r="G151" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6265,14 +6334,14 @@
         <v>451</v>
       </c>
       <c r="D152" s="29">
-        <v>52.78</v>
+        <v>614.17</v>
       </c>
       <c r="E152" s="30">
         <v>0</v>
       </c>
       <c r="F152" s="31">
         <f t="shared" si="8"/>
-        <v>-52.78</v>
+        <v>-614.17</v>
       </c>
       <c r="G152" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6291,14 +6360,14 @@
         <v>454</v>
       </c>
       <c r="D153" s="29">
-        <v>530.91</v>
+        <v>49.26</v>
       </c>
       <c r="E153" s="30">
         <v>0</v>
       </c>
       <c r="F153" s="31">
         <f t="shared" si="8"/>
-        <v>-530.91</v>
+        <v>-49.26</v>
       </c>
       <c r="G153" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6317,14 +6386,14 @@
         <v>457</v>
       </c>
       <c r="D154" s="29">
-        <v>722</v>
+        <v>14322.49</v>
       </c>
       <c r="E154" s="30">
         <v>0</v>
       </c>
       <c r="F154" s="31">
         <f t="shared" si="8"/>
-        <v>-722</v>
+        <v>-14322.49</v>
       </c>
       <c r="G154" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6343,14 +6412,14 @@
         <v>460</v>
       </c>
       <c r="D155" s="29">
-        <v>64.64</v>
+        <v>41431.12</v>
       </c>
       <c r="E155" s="30">
         <v>0</v>
       </c>
       <c r="F155" s="31">
         <f t="shared" si="8"/>
-        <v>-64.64</v>
+        <v>-41431.12</v>
       </c>
       <c r="G155" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6369,14 +6438,14 @@
         <v>463</v>
       </c>
       <c r="D156" s="29">
-        <v>4169.85</v>
+        <v>11004.68</v>
       </c>
       <c r="E156" s="30">
         <v>0</v>
       </c>
       <c r="F156" s="31">
         <f t="shared" si="8"/>
-        <v>-4169.85</v>
+        <v>-11004.68</v>
       </c>
       <c r="G156" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6395,14 +6464,14 @@
         <v>466</v>
       </c>
       <c r="D157" s="29">
-        <v>71771.44</v>
+        <v>352.78000000000003</v>
       </c>
       <c r="E157" s="30">
         <v>0</v>
       </c>
       <c r="F157" s="31">
         <f t="shared" si="8"/>
-        <v>-71771.44</v>
+        <v>-352.78000000000003</v>
       </c>
       <c r="G157" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6421,14 +6490,14 @@
         <v>469</v>
       </c>
       <c r="D158" s="29">
-        <v>0.19</v>
+        <v>710.91</v>
       </c>
       <c r="E158" s="30">
         <v>0</v>
       </c>
       <c r="F158" s="31">
         <f t="shared" si="8"/>
-        <v>-0.19</v>
+        <v>-710.91</v>
       </c>
       <c r="G158" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6447,14 +6516,14 @@
         <v>472</v>
       </c>
       <c r="D159" s="29">
-        <v>3342.15</v>
+        <v>1257</v>
       </c>
       <c r="E159" s="30">
         <v>0</v>
       </c>
       <c r="F159" s="31">
         <f t="shared" si="8"/>
-        <v>-3342.15</v>
+        <v>-1257</v>
       </c>
       <c r="G159" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6473,14 +6542,14 @@
         <v>475</v>
       </c>
       <c r="D160" s="29">
-        <v>0.86</v>
+        <v>564.64</v>
       </c>
       <c r="E160" s="30">
         <v>0</v>
       </c>
       <c r="F160" s="31">
         <f t="shared" si="8"/>
-        <v>-0.86</v>
+        <v>-564.64</v>
       </c>
       <c r="G160" s="32" t="str">
         <f t="shared" si="9"/>
@@ -6488,40 +6557,170 @@
       </c>
       <c r="H160" s="33"/>
     </row>
-    <row r="161" ht="31.9" customHeight="1" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="35" t="s">
+    <row r="161" ht="52.9" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A161" s="26" t="s">
         <v>476</v>
       </c>
-      <c r="B161" s="36"/>
-      <c r="C161" s="37"/>
-      <c r="D161" s="38">
-        <f>SUM(D8:D160)</f>
-        <v>5245979.3100000005</v>
-      </c>
-      <c r="E161" s="39">
-        <f>SUM(E8:E160)</f>
-        <v>0</v>
-      </c>
-      <c r="F161" s="40">
-        <f>SUM(F8:F160)</f>
-        <v>-5245979.3100000005</v>
-      </c>
-      <c r="G161" s="41" t="str">
+      <c r="B161" s="27" t="s">
+        <v>477</v>
+      </c>
+      <c r="C161" s="28" t="s">
+        <v>478</v>
+      </c>
+      <c r="D161" s="29">
+        <v>6169.85</v>
+      </c>
+      <c r="E161" s="30">
+        <v>0</v>
+      </c>
+      <c r="F161" s="31">
+        <f t="shared" si="8"/>
+        <v>-6169.85</v>
+      </c>
+      <c r="G161" s="32" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="H161" s="42"/>
-    </row>
-    <row r="162" ht="27.6" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="43" t="s">
-        <v>477</v>
-      </c>
-      <c r="B162" s="43"/>
-      <c r="F162" s="43" t="s">
-        <v>478</v>
-      </c>
-      <c r="G162" s="44"/>
-      <c r="H162" s="45"/>
+      <c r="H161" s="33"/>
+    </row>
+    <row r="162" ht="52.9" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A162" s="26" t="s">
+        <v>479</v>
+      </c>
+      <c r="B162" s="27" t="s">
+        <v>480</v>
+      </c>
+      <c r="C162" s="28" t="s">
+        <v>481</v>
+      </c>
+      <c r="D162" s="29">
+        <v>151146.44</v>
+      </c>
+      <c r="E162" s="30">
+        <v>0</v>
+      </c>
+      <c r="F162" s="31">
+        <f t="shared" si="8"/>
+        <v>-151146.44</v>
+      </c>
+      <c r="G162" s="32" t="str">
+        <f t="shared" si="9"/>
+        <v>-</v>
+      </c>
+      <c r="H162" s="33"/>
+    </row>
+    <row r="163" ht="52.9" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A163" s="26" t="s">
+        <v>482</v>
+      </c>
+      <c r="B163" s="27" t="s">
+        <v>483</v>
+      </c>
+      <c r="C163" s="28" t="s">
+        <v>484</v>
+      </c>
+      <c r="D163" s="29">
+        <v>0.19</v>
+      </c>
+      <c r="E163" s="30">
+        <v>0</v>
+      </c>
+      <c r="F163" s="31">
+        <f t="shared" si="8"/>
+        <v>-0.19</v>
+      </c>
+      <c r="G163" s="32" t="str">
+        <f t="shared" si="9"/>
+        <v>-</v>
+      </c>
+      <c r="H163" s="33"/>
+    </row>
+    <row r="164" ht="52.9" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A164" s="26" t="s">
+        <v>485</v>
+      </c>
+      <c r="B164" s="27" t="s">
+        <v>486</v>
+      </c>
+      <c r="C164" s="28" t="s">
+        <v>487</v>
+      </c>
+      <c r="D164" s="29">
+        <v>4692.150000000001</v>
+      </c>
+      <c r="E164" s="30">
+        <v>0</v>
+      </c>
+      <c r="F164" s="31">
+        <f t="shared" si="8"/>
+        <v>-4692.150000000001</v>
+      </c>
+      <c r="G164" s="32" t="str">
+        <f t="shared" si="9"/>
+        <v>-</v>
+      </c>
+      <c r="H164" s="33"/>
+    </row>
+    <row r="165" ht="52.9" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A165" s="26" t="s">
+        <v>488</v>
+      </c>
+      <c r="B165" s="27" t="s">
+        <v>489</v>
+      </c>
+      <c r="C165" s="28" t="s">
+        <v>490</v>
+      </c>
+      <c r="D165" s="29">
+        <v>0.86</v>
+      </c>
+      <c r="E165" s="30">
+        <v>0</v>
+      </c>
+      <c r="F165" s="31">
+        <f t="shared" si="8"/>
+        <v>-0.86</v>
+      </c>
+      <c r="G165" s="32" t="str">
+        <f t="shared" si="9"/>
+        <v>-</v>
+      </c>
+      <c r="H165" s="33"/>
+    </row>
+    <row r="166" ht="31.9" customHeight="1" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="35" t="s">
+        <v>491</v>
+      </c>
+      <c r="B166" s="36"/>
+      <c r="C166" s="37"/>
+      <c r="D166" s="38">
+        <f>SUM(D8:D165)</f>
+        <v>12775218.178860003</v>
+      </c>
+      <c r="E166" s="39">
+        <f>SUM(E8:E165)</f>
+        <v>0</v>
+      </c>
+      <c r="F166" s="40">
+        <f>SUM(F8:F165)</f>
+        <v>-12775218.178860003</v>
+      </c>
+      <c r="G166" s="41" t="str">
+        <f t="shared" si="9"/>
+        <v>-</v>
+      </c>
+      <c r="H166" s="42"/>
+    </row>
+    <row r="167" ht="27.6" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="43" t="s">
+        <v>492</v>
+      </c>
+      <c r="B167" s="43"/>
+      <c r="F167" s="43" t="s">
+        <v>493</v>
+      </c>
+      <c r="G167" s="44"/>
+      <c r="H167" s="45"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>